<commit_message>
add logger and point with choose state.json file
</commit_message>
<xml_diff>
--- a/table_after_parsing/parsing_28_04_2024.xlsx
+++ b/table_after_parsing/parsing_28_04_2024.xlsx
@@ -817,7 +817,13 @@
           <t>Краснодарский край, Краснодар</t>
         </is>
       </c>
-      <c r="B8" s="4" t="n"/>
+      <c r="B8" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">окна пвх - 153
+пластиковые окна - 4781
+</t>
+        </is>
+      </c>
       <c r="C8" s="5" t="n">
         <v>17653</v>
       </c>
@@ -841,7 +847,13 @@
           <t>Краснодарский край, Сочи</t>
         </is>
       </c>
-      <c r="B9" s="4" t="n"/>
+      <c r="B9" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">окна пвх - 29
+пластиковые окна - 1260
+</t>
+        </is>
+      </c>
       <c r="C9" s="6" t="n">
         <v>9607</v>
       </c>
@@ -865,7 +877,13 @@
           <t>Краснодарский край, Ейск</t>
         </is>
       </c>
-      <c r="B10" s="4" t="n"/>
+      <c r="B10" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">окна пвх - 17
+пластиковые окна - 296
+</t>
+        </is>
+      </c>
       <c r="C10" s="6" t="n">
         <v>702</v>
       </c>
@@ -889,7 +907,13 @@
           <t>Краснодарский край, Геленджик</t>
         </is>
       </c>
-      <c r="B11" s="4" t="n"/>
+      <c r="B11" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">окна пвх - 14
+пластиковые окна - 300
+</t>
+        </is>
+      </c>
       <c r="C11" s="6" t="n">
         <v>1891</v>
       </c>
@@ -913,7 +937,13 @@
           <t>Краснодарский край, Кропоткин</t>
         </is>
       </c>
-      <c r="B12" s="4" t="n"/>
+      <c r="B12" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">окна пвх - 4
+пластиковые окна - 257
+</t>
+        </is>
+      </c>
       <c r="C12" s="6" t="n">
         <v>467</v>
       </c>
@@ -937,7 +967,13 @@
           <t>Краснодарский край, Славянск-на-Кубани</t>
         </is>
       </c>
-      <c r="B13" s="4" t="n"/>
+      <c r="B13" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">окна пвх - 11
+пластиковые окна - 254
+</t>
+        </is>
+      </c>
       <c r="C13" s="6" t="n">
         <v>677</v>
       </c>
@@ -961,7 +997,13 @@
           <t>Краснодарский край, Туапсе</t>
         </is>
       </c>
-      <c r="B14" s="4" t="n"/>
+      <c r="B14" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">окна пвх - 7
+пластиковые окна - 226
+</t>
+        </is>
+      </c>
       <c r="C14" s="6" t="n">
         <v>539</v>
       </c>
@@ -985,7 +1027,13 @@
           <t>Краснодарский край, Лабинск</t>
         </is>
       </c>
-      <c r="B15" s="4" t="n"/>
+      <c r="B15" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">окна пвх - 1
+пластиковые окна - 173
+</t>
+        </is>
+      </c>
       <c r="C15" s="6" t="n">
         <v>454</v>
       </c>
@@ -1009,7 +1057,13 @@
           <t>Краснодарский край, Белореченск</t>
         </is>
       </c>
-      <c r="B16" s="4" t="n"/>
+      <c r="B16" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">окна пвх - 6
+пластиковые окна - 265
+</t>
+        </is>
+      </c>
       <c r="C16" s="6" t="n">
         <v>540</v>
       </c>
@@ -1033,7 +1087,13 @@
           <t>Краснодарский край, Тихорецк</t>
         </is>
       </c>
-      <c r="B17" s="4" t="n"/>
+      <c r="B17" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">окна пвх - 3
+пластиковые окна - 210
+</t>
+        </is>
+      </c>
       <c r="C17" s="6" t="n">
         <v>832</v>
       </c>
@@ -1057,7 +1117,13 @@
           <t>Краснодарский край, Крымск</t>
         </is>
       </c>
-      <c r="B18" s="4" t="n"/>
+      <c r="B18" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">окна пвх - 11
+пластиковые окна - 231
+</t>
+        </is>
+      </c>
       <c r="C18" s="6" t="n">
         <v>403</v>
       </c>
@@ -1081,7 +1147,13 @@
           <t>Краснодарский край, Тимашёвск</t>
         </is>
       </c>
-      <c r="B19" s="4" t="n"/>
+      <c r="B19" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">окна пвх - 3
+пластиковые окна - 190
+</t>
+        </is>
+      </c>
       <c r="C19" s="6" t="n">
         <v>265</v>
       </c>
@@ -1105,7 +1177,13 @@
           <t>Краснодарский край, Каневская</t>
         </is>
       </c>
-      <c r="B20" s="4" t="n"/>
+      <c r="B20" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">окна пвх - 1
+пластиковые окна - 121
+</t>
+        </is>
+      </c>
       <c r="C20" s="6" t="n">
         <v>76</v>
       </c>
@@ -1153,7 +1231,13 @@
           <t>Краснодарский край, Горячий Ключ</t>
         </is>
       </c>
-      <c r="B22" s="4" t="n"/>
+      <c r="B22" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">окна пвх - 3
+пластиковые окна - 130
+</t>
+        </is>
+      </c>
       <c r="C22" s="6" t="n">
         <v>822</v>
       </c>
@@ -1177,7 +1261,13 @@
           <t>Краснодарский край, Усть-Лабинск</t>
         </is>
       </c>
-      <c r="B23" s="4" t="n"/>
+      <c r="B23" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">окна пвх - 6
+пластиковые окна - 142
+</t>
+        </is>
+      </c>
       <c r="C23" s="6" t="n">
         <v>812</v>
       </c>
@@ -1201,7 +1291,13 @@
           <t>Краснодарский край, Абинск</t>
         </is>
       </c>
-      <c r="B24" s="4" t="n"/>
+      <c r="B24" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">окна пвх - 2
+пластиковые окна - 77
+</t>
+        </is>
+      </c>
       <c r="C24" s="6" t="n">
         <v>382</v>
       </c>
@@ -1225,7 +1321,13 @@
           <t>Краснодарский край, Ленинградская</t>
         </is>
       </c>
-      <c r="B25" s="4" t="n"/>
+      <c r="B25" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">окна пвх - 0
+пластиковые окна - 64
+</t>
+        </is>
+      </c>
       <c r="C25" s="6" t="n">
         <v>42</v>
       </c>
@@ -1249,7 +1351,13 @@
           <t>Краснодарский край, Динская</t>
         </is>
       </c>
-      <c r="B26" s="4" t="n"/>
+      <c r="B26" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">окна пвх - 2
+пластиковые окна - 91
+</t>
+        </is>
+      </c>
       <c r="C26" s="6" t="n">
         <v>249</v>
       </c>
@@ -1273,7 +1381,13 @@
           <t>Краснодарский край, Гулькевичи</t>
         </is>
       </c>
-      <c r="B27" s="4" t="n"/>
+      <c r="B27" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">окна пвх - 1
+пластиковые окна - 98
+</t>
+        </is>
+      </c>
       <c r="C27" s="6" t="n">
         <v>336</v>
       </c>
@@ -1297,7 +1411,13 @@
           <t>Краснодарский край, Павловская</t>
         </is>
       </c>
-      <c r="B28" s="4" t="n"/>
+      <c r="B28" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">окна пвх - 1
+пластиковые окна - 79
+</t>
+        </is>
+      </c>
       <c r="C28" s="6" t="n">
         <v>53</v>
       </c>
@@ -1321,7 +1441,13 @@
           <t>Краснодарский край, Приморско-Ахтарск</t>
         </is>
       </c>
-      <c r="B29" s="4" t="n"/>
+      <c r="B29" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">окна пвх - 1
+пластиковые окна - 63
+</t>
+        </is>
+      </c>
       <c r="C29" s="6" t="n">
         <v>52</v>
       </c>
@@ -1345,7 +1471,13 @@
           <t>Краснодарский край, Староминская</t>
         </is>
       </c>
-      <c r="B30" s="4" t="n"/>
+      <c r="B30" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">окна пвх - 0
+пластиковые окна - 60
+</t>
+        </is>
+      </c>
       <c r="C30" s="6" t="n">
         <v>29</v>
       </c>
@@ -1369,7 +1501,13 @@
           <t>Краснодарский край, Кущёвская</t>
         </is>
       </c>
-      <c r="B31" s="4" t="n"/>
+      <c r="B31" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">окна пвх - 1
+пластиковые окна - 89
+</t>
+        </is>
+      </c>
       <c r="C31" s="6" t="n">
         <v>48</v>
       </c>
@@ -1393,7 +1531,13 @@
           <t>Краснодарский край, Полтавская</t>
         </is>
       </c>
-      <c r="B32" s="4" t="n"/>
+      <c r="B32" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">окна пвх - 2
+пластиковые окна - 53
+</t>
+        </is>
+      </c>
       <c r="C32" s="6" t="n">
         <v>22</v>
       </c>
@@ -1417,7 +1561,13 @@
           <t>Краснодарский край, Мостовской</t>
         </is>
       </c>
-      <c r="B33" s="4" t="n"/>
+      <c r="B33" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">окна пвх - 2
+пластиковые окна - 48
+</t>
+        </is>
+      </c>
       <c r="C33" s="6" t="n">
         <v>274</v>
       </c>
@@ -1441,7 +1591,13 @@
           <t>Краснодарский край, Тбилисская</t>
         </is>
       </c>
-      <c r="B34" s="4" t="n"/>
+      <c r="B34" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">окна пвх - 0
+пластиковые окна - 51
+</t>
+        </is>
+      </c>
       <c r="C34" s="6" t="n">
         <v>96</v>
       </c>
@@ -1465,7 +1621,13 @@
           <t>Краснодарский край, Ильский</t>
         </is>
       </c>
-      <c r="B35" s="4" t="n"/>
+      <c r="B35" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">окна пвх - 0
+пластиковые окна - 42
+</t>
+        </is>
+      </c>
       <c r="C35" s="6" t="n">
         <v>83</v>
       </c>
@@ -1489,7 +1651,13 @@
           <t>Краснодарский край, Северская</t>
         </is>
       </c>
-      <c r="B36" s="4" t="n"/>
+      <c r="B36" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">окна пвх - 1
+пластиковые окна - 45
+</t>
+        </is>
+      </c>
       <c r="C36" s="6" t="n">
         <v>316</v>
       </c>
@@ -1513,7 +1681,13 @@
           <t>Краснодарский край, Елизаветинская</t>
         </is>
       </c>
-      <c r="B37" s="4" t="n"/>
+      <c r="B37" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">окна пвх - 0
+пластиковые окна - 31
+</t>
+        </is>
+      </c>
       <c r="C37" s="6" t="n">
         <v>69</v>
       </c>
@@ -1537,7 +1711,13 @@
           <t>Краснодарский край, Новотитаровская</t>
         </is>
       </c>
-      <c r="B38" s="4" t="n"/>
+      <c r="B38" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">окна пвх - 0
+пластиковые окна - 44
+</t>
+        </is>
+      </c>
       <c r="C38" s="6" t="n">
         <v>227</v>
       </c>
@@ -1561,7 +1741,13 @@
           <t>Краснодарский край, Афипский</t>
         </is>
       </c>
-      <c r="B39" s="4" t="n"/>
+      <c r="B39" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">окна пвх - 1
+пластиковые окна - 41
+</t>
+        </is>
+      </c>
       <c r="C39" s="6" t="n">
         <v>48</v>
       </c>
@@ -1585,7 +1771,13 @@
           <t>Краснодарский край, Брюховецкая</t>
         </is>
       </c>
-      <c r="B40" s="4" t="n"/>
+      <c r="B40" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">окна пвх - 4
+пластиковые окна - 60
+</t>
+        </is>
+      </c>
       <c r="C40" s="6" t="n">
         <v>41</v>
       </c>
@@ -1609,7 +1801,13 @@
           <t>Краснодарский край, Ахтырский</t>
         </is>
       </c>
-      <c r="B41" s="4" t="n"/>
+      <c r="B41" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">окна пвх - 0
+пластиковые окна - 20
+</t>
+        </is>
+      </c>
       <c r="C41" s="6" t="n">
         <v>16</v>
       </c>
@@ -1633,7 +1831,13 @@
           <t>Краснодарский край, Новопокровская</t>
         </is>
       </c>
-      <c r="B42" s="4" t="n"/>
+      <c r="B42" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">окна пвх - 0
+пластиковые окна - 18
+</t>
+        </is>
+      </c>
       <c r="C42" s="6" t="n">
         <v>36</v>
       </c>
@@ -1657,7 +1861,13 @@
           <t>Краснодарский край, Выселки</t>
         </is>
       </c>
-      <c r="B43" s="4" t="n"/>
+      <c r="B43" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">окна пвх - 0
+пластиковые окна - 46
+</t>
+        </is>
+      </c>
       <c r="C43" s="6" t="n">
         <v>136</v>
       </c>
@@ -1681,7 +1891,13 @@
           <t>Краснодарский край, Старощербиновская</t>
         </is>
       </c>
-      <c r="B44" s="4" t="n"/>
+      <c r="B44" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">окна пвх - 1
+пластиковые окна - 38
+</t>
+        </is>
+      </c>
       <c r="C44" s="6" t="n">
         <v>20</v>
       </c>
@@ -1705,7 +1921,13 @@
           <t>Краснодарский край, Холмская</t>
         </is>
       </c>
-      <c r="B45" s="4" t="n"/>
+      <c r="B45" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">окна пвх - 0
+пластиковые окна - 24
+</t>
+        </is>
+      </c>
       <c r="C45" s="6" t="n">
         <v>56</v>
       </c>
@@ -1729,7 +1951,13 @@
           <t>Краснодарский край, Белая Глина</t>
         </is>
       </c>
-      <c r="B46" s="4" t="n"/>
+      <c r="B46" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">окна пвх - 0
+пластиковые окна - 36
+</t>
+        </is>
+      </c>
       <c r="C46" s="6" t="n">
         <v>20</v>
       </c>
@@ -1753,7 +1981,13 @@
           <t>Краснодарский край, Медведовская</t>
         </is>
       </c>
-      <c r="B47" s="4" t="n"/>
+      <c r="B47" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">окна пвх - 0
+пластиковые окна - 25
+</t>
+        </is>
+      </c>
       <c r="C47" s="6" t="n">
         <v>33</v>
       </c>
@@ -1777,7 +2011,13 @@
           <t>Краснодарский край, Ладожская</t>
         </is>
       </c>
-      <c r="B48" s="4" t="n"/>
+      <c r="B48" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">окна пвх - 0
+пластиковые окна - 14
+</t>
+        </is>
+      </c>
       <c r="C48" s="6" t="n">
         <v>104</v>
       </c>
@@ -1801,7 +2041,13 @@
           <t>Краснодарский край, Крыловская</t>
         </is>
       </c>
-      <c r="B49" s="4" t="n"/>
+      <c r="B49" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">окна пвх - 0
+пластиковые окна - 26
+</t>
+        </is>
+      </c>
       <c r="C49" s="6" t="n">
         <v>12</v>
       </c>
@@ -1825,7 +2071,13 @@
           <t>Краснодарский край, Старовеличковская</t>
         </is>
       </c>
-      <c r="B50" s="4" t="n"/>
+      <c r="B50" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">окна пвх - 0
+пластиковые окна - 10
+</t>
+        </is>
+      </c>
       <c r="C50" s="6" t="n">
         <v>31</v>
       </c>
@@ -1849,7 +2101,13 @@
           <t>Краснодарский край, Калининская</t>
         </is>
       </c>
-      <c r="B51" s="4" t="n"/>
+      <c r="B51" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">окна пвх - 0
+пластиковые окна - 19
+</t>
+        </is>
+      </c>
       <c r="C51" s="6" t="n">
         <v>116</v>
       </c>
@@ -1873,7 +2131,13 @@
           <t>Краснодарский край, Васюринская</t>
         </is>
       </c>
-      <c r="B52" s="4" t="n"/>
+      <c r="B52" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">окна пвх - 2
+пластиковые окна - 17
+</t>
+        </is>
+      </c>
       <c r="C52" s="6" t="n">
         <v>41</v>
       </c>
@@ -1897,7 +2161,13 @@
           <t>Краснодарский край, Стародеревянковская</t>
         </is>
       </c>
-      <c r="B53" s="4" t="n"/>
+      <c r="B53" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">окна пвх - 0
+пластиковые окна - 4
+</t>
+        </is>
+      </c>
       <c r="C53" s="6" t="n">
         <v>8</v>
       </c>
@@ -1949,7 +2219,13 @@
           <t>Краснодарский край, Новоминская</t>
         </is>
       </c>
-      <c r="B55" s="4" t="n"/>
+      <c r="B55" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">окна пвх - 1
+пластиковые окна - 8
+</t>
+        </is>
+      </c>
       <c r="C55" s="6" t="n">
         <v>9</v>
       </c>
@@ -1973,7 +2249,13 @@
           <t>Краснодарский край, Кавказская</t>
         </is>
       </c>
-      <c r="B56" s="4" t="n"/>
+      <c r="B56" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">окна пвх - 0
+пластиковые окна - 7
+</t>
+        </is>
+      </c>
       <c r="C56" s="6" t="n">
         <v>91</v>
       </c>
@@ -1997,7 +2279,13 @@
           <t>Краснодарский край, Псебай</t>
         </is>
       </c>
-      <c r="B57" s="4" t="n"/>
+      <c r="B57" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">окна пвх - 0
+пластиковые окна - 11
+</t>
+        </is>
+      </c>
       <c r="C57" s="6" t="n">
         <v>16</v>
       </c>
@@ -2021,7 +2309,13 @@
           <t>Краснодарский край, Марьянская</t>
         </is>
       </c>
-      <c r="B58" s="4" t="n"/>
+      <c r="B58" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">окна пвх - 1
+пластиковые окна - 8
+</t>
+        </is>
+      </c>
       <c r="C58" s="6" t="n">
         <v>85</v>
       </c>
@@ -2045,7 +2339,13 @@
           <t>Краснодарский край, Старомышастовская</t>
         </is>
       </c>
-      <c r="B59" s="4" t="n"/>
+      <c r="B59" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">окна пвх - 0
+пластиковые окна - 6
+</t>
+        </is>
+      </c>
       <c r="C59" s="6" t="n">
         <v>6</v>
       </c>
@@ -2069,7 +2369,13 @@
           <t>Краснодарский край, Анастасиевская</t>
         </is>
       </c>
-      <c r="B60" s="4" t="n"/>
+      <c r="B60" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">окна пвх - 0
+пластиковые окна - 9
+</t>
+        </is>
+      </c>
       <c r="C60" s="6" t="n">
         <v>15</v>
       </c>
@@ -2093,7 +2399,13 @@
           <t>Краснодарский край, Пластуновская</t>
         </is>
       </c>
-      <c r="B61" s="4" t="n"/>
+      <c r="B61" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">окна пвх - 0
+пластиковые окна - 7
+</t>
+        </is>
+      </c>
       <c r="C61" s="6" t="n">
         <v>37</v>
       </c>
@@ -2117,7 +2429,13 @@
           <t>Краснодарский край, Старонижестеблиевская</t>
         </is>
       </c>
-      <c r="B62" s="4" t="n"/>
+      <c r="B62" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">окна пвх - 0
+пластиковые окна - 6
+</t>
+        </is>
+      </c>
       <c r="C62" s="6" t="n">
         <v>5</v>
       </c>
@@ -2141,7 +2459,13 @@
           <t>Краснодарский край, Новомихайловский</t>
         </is>
       </c>
-      <c r="B63" s="4" t="n"/>
+      <c r="B63" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">окна пвх - 0
+пластиковые окна - 15
+</t>
+        </is>
+      </c>
       <c r="C63" s="6" t="n">
         <v>17</v>
       </c>
@@ -2165,7 +2489,13 @@
           <t>Краснодарский край, Новомышастовская</t>
         </is>
       </c>
-      <c r="B64" s="4" t="n"/>
+      <c r="B64" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">окна пвх - 1
+пластиковые окна - 5
+</t>
+        </is>
+      </c>
       <c r="C64" s="6" t="n">
         <v>40</v>
       </c>
@@ -2189,7 +2519,13 @@
           <t>Краснодарский край, Трудобеликовский</t>
         </is>
       </c>
-      <c r="B65" s="4" t="n"/>
+      <c r="B65" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">окна пвх - 0
+пластиковые окна - 6
+</t>
+        </is>
+      </c>
       <c r="C65" s="6" t="n">
         <v>4</v>
       </c>
@@ -2213,7 +2549,13 @@
           <t>Краснодарский край, Нововеличковская</t>
         </is>
       </c>
-      <c r="B66" s="4" t="n"/>
+      <c r="B66" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">окна пвх - 0
+пластиковые окна - 6
+</t>
+        </is>
+      </c>
       <c r="C66" s="6" t="n">
         <v>22</v>
       </c>
@@ -2237,7 +2579,13 @@
           <t>Краснодарский край, Архангельская</t>
         </is>
       </c>
-      <c r="B67" s="4" t="n"/>
+      <c r="B67" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">окна пвх - 0
+пластиковые окна - 7
+</t>
+        </is>
+      </c>
       <c r="C67" s="6" t="n">
         <v>62</v>
       </c>
@@ -2261,7 +2609,13 @@
           <t>Краснодарский край, Черноморский</t>
         </is>
       </c>
-      <c r="B68" s="4" t="n"/>
+      <c r="B68" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">окна пвх - 0
+пластиковые окна - 2
+</t>
+        </is>
+      </c>
       <c r="C68" s="6" t="n">
         <v>4</v>
       </c>
@@ -2285,7 +2639,13 @@
           <t>Краснодарский край, Фастовецкая</t>
         </is>
       </c>
-      <c r="B69" s="4" t="n"/>
+      <c r="B69" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">окна пвх - 0
+пластиковые окна - 1
+</t>
+        </is>
+      </c>
       <c r="C69" s="6" t="n">
         <v>2</v>
       </c>
@@ -2309,7 +2669,13 @@
           <t>Краснодарский край, Воронежская</t>
         </is>
       </c>
-      <c r="B70" s="4" t="n"/>
+      <c r="B70" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">окна пвх - 0
+пластиковые окна - 3
+</t>
+        </is>
+      </c>
       <c r="C70" s="6" t="n">
         <v>9</v>
       </c>
@@ -2333,7 +2699,13 @@
           <t>Краснодарский край, Переясловская</t>
         </is>
       </c>
-      <c r="B71" s="4" t="n"/>
+      <c r="B71" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">окна пвх - 0
+пластиковые окна - 3
+</t>
+        </is>
+      </c>
       <c r="C71" s="6" t="n">
         <v>3</v>
       </c>
@@ -2357,7 +2729,13 @@
           <t>Краснодарский край, Роговская</t>
         </is>
       </c>
-      <c r="B72" s="4" t="n"/>
+      <c r="B72" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">окна пвх - 0
+пластиковые окна - 6
+</t>
+        </is>
+      </c>
       <c r="C72" s="6" t="n">
         <v>6</v>
       </c>
@@ -2381,7 +2759,13 @@
           <t>Краснодарский край, Архипо-Осиповка</t>
         </is>
       </c>
-      <c r="B73" s="4" t="n"/>
+      <c r="B73" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">окна пвх - 0
+пластиковые окна - 28
+</t>
+        </is>
+      </c>
       <c r="C73" s="6" t="n">
         <v>38</v>
       </c>
@@ -2405,7 +2789,13 @@
           <t>Краснодарский край, Смоленская</t>
         </is>
       </c>
-      <c r="B74" s="4" t="n"/>
+      <c r="B74" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">окна пвх - 0
+пластиковые окна - 2
+</t>
+        </is>
+      </c>
       <c r="C74" s="6" t="n">
         <v>4</v>
       </c>
@@ -2429,7 +2819,13 @@
           <t>Краснодарский край, Кабардинка</t>
         </is>
       </c>
-      <c r="B75" s="4" t="n"/>
+      <c r="B75" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">окна пвх - 2
+пластиковые окна - 27
+</t>
+        </is>
+      </c>
       <c r="C75" s="6" t="n">
         <v>102</v>
       </c>
@@ -2453,7 +2849,13 @@
           <t>Краснодарский край, Темиргоевская</t>
         </is>
       </c>
-      <c r="B76" s="4" t="n"/>
+      <c r="B76" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">окна пвх - 2
+пластиковые окна - 8
+</t>
+        </is>
+      </c>
       <c r="C76" s="6" t="n">
         <v>6</v>
       </c>
@@ -2501,7 +2903,13 @@
           <t>Краснодарский край, Джубга</t>
         </is>
       </c>
-      <c r="B78" s="4" t="n"/>
+      <c r="B78" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">окна пвх - 0
+пластиковые окна - 27
+</t>
+        </is>
+      </c>
       <c r="C78" s="6" t="n">
         <v>40</v>
       </c>
@@ -2525,7 +2933,13 @@
           <t>Краснодарский край, Новодеревянковская</t>
         </is>
       </c>
-      <c r="B79" s="4" t="n"/>
+      <c r="B79" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">окна пвх - 0
+пластиковые окна - 3
+</t>
+        </is>
+      </c>
       <c r="C79" s="6" t="n">
         <v>3</v>
       </c>
@@ -2569,7 +2983,13 @@
           <t>Краснодарский край, Новорождественская</t>
         </is>
       </c>
-      <c r="B81" s="4" t="n"/>
+      <c r="B81" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">окна пвх - 0
+пластиковые окна - 3
+</t>
+        </is>
+      </c>
       <c r="C81" s="6" t="n">
         <v>2</v>
       </c>
@@ -2593,7 +3013,13 @@
           <t>Краснодарский край, Новолеушковская</t>
         </is>
       </c>
-      <c r="B82" s="4" t="n"/>
+      <c r="B82" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">окна пвх - 0
+пластиковые окна - 3
+</t>
+        </is>
+      </c>
       <c r="C82" s="6" t="n">
         <v>17</v>
       </c>
@@ -2645,7 +3071,13 @@
           <t>Краснодарский край, Новомалороссийская</t>
         </is>
       </c>
-      <c r="B84" s="4" t="n"/>
+      <c r="B84" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">окна пвх - 0
+пластиковые окна - 3
+</t>
+        </is>
+      </c>
       <c r="C84" s="6" t="n">
         <v>5</v>
       </c>
@@ -2669,7 +3101,13 @@
           <t>Краснодарский край, Калниболотская</t>
         </is>
       </c>
-      <c r="B85" s="4" t="n"/>
+      <c r="B85" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">окна пвх - 0
+пластиковые окна - 1
+</t>
+        </is>
+      </c>
       <c r="C85" s="6" t="n">
         <v>4</v>
       </c>
@@ -2693,7 +3131,13 @@
           <t>Краснодарский край, Кирпильская</t>
         </is>
       </c>
-      <c r="B86" s="4" t="n"/>
+      <c r="B86" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">окна пвх - 0
+пластиковые окна - 7
+</t>
+        </is>
+      </c>
       <c r="C86" s="6" t="n">
         <v>37</v>
       </c>
@@ -2717,7 +3161,13 @@
           <t>Краснодарский край, Старолеушковская</t>
         </is>
       </c>
-      <c r="B87" s="4" t="n"/>
+      <c r="B87" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">окна пвх - 0
+пластиковые окна - 2
+</t>
+        </is>
+      </c>
       <c r="C87" s="6" t="n">
         <v>1</v>
       </c>
@@ -2741,7 +3191,13 @@
           <t>Краснодарский край, Южный</t>
         </is>
       </c>
-      <c r="B88" s="4" t="n"/>
+      <c r="B88" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">окна пвх - 0
+пластиковые окна - 5
+</t>
+        </is>
+      </c>
       <c r="C88" s="6" t="n">
         <v>73</v>
       </c>
@@ -2765,7 +3221,13 @@
           <t>Краснодарский край, Мингрельская</t>
         </is>
       </c>
-      <c r="B89" s="4" t="n"/>
+      <c r="B89" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">окна пвх - 0
+пластиковые окна - 5
+</t>
+        </is>
+      </c>
       <c r="C89" s="6" t="n">
         <v>22</v>
       </c>
@@ -2789,7 +3251,13 @@
           <t>Краснодарский край, Новоджерелиевская</t>
         </is>
       </c>
-      <c r="B90" s="4" t="n"/>
+      <c r="B90" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">окна пвх - 0
+пластиковые окна - 2
+</t>
+        </is>
+      </c>
       <c r="C90" s="6" t="n">
         <v>6</v>
       </c>
@@ -2813,7 +3281,13 @@
           <t>Краснодарский край, Новокорсунская</t>
         </is>
       </c>
-      <c r="B91" s="4" t="n"/>
+      <c r="B91" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">окна пвх - 0
+пластиковые окна - 3
+</t>
+        </is>
+      </c>
       <c r="C91" s="6" t="n">
         <v>5</v>
       </c>
@@ -2837,7 +3311,13 @@
           <t>Краснодарский край, Ольгинская</t>
         </is>
       </c>
-      <c r="B92" s="4" t="n"/>
+      <c r="B92" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">окна пвх - 0
+пластиковые окна - 1
+</t>
+        </is>
+      </c>
       <c r="C92" s="6" t="n">
         <v>6</v>
       </c>
@@ -2885,7 +3365,13 @@
           <t>Краснодарский край, Азовская</t>
         </is>
       </c>
-      <c r="B94" s="4" t="n"/>
+      <c r="B94" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">окна пвх - 0
+пластиковые окна - 2
+</t>
+        </is>
+      </c>
       <c r="C94" s="6" t="n">
         <v>1</v>
       </c>
@@ -2909,7 +3395,13 @@
           <t>Краснодарский край, Небуг</t>
         </is>
       </c>
-      <c r="B95" s="4" t="n"/>
+      <c r="B95" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">окна пвх - 0
+пластиковые окна - 11
+</t>
+        </is>
+      </c>
       <c r="C95" s="6" t="n">
         <v>25</v>
       </c>
@@ -2933,7 +3425,13 @@
           <t>Краснодарский край, Агроном</t>
         </is>
       </c>
-      <c r="B96" s="4" t="n"/>
+      <c r="B96" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">окна пвх - 0
+пластиковые окна - 4
+</t>
+        </is>
+      </c>
       <c r="C96" s="6" t="n">
         <v>37</v>
       </c>
@@ -3001,7 +3499,13 @@
           <t>Краснодарский край, Новоплатнировская</t>
         </is>
       </c>
-      <c r="B99" s="4" t="n"/>
+      <c r="B99" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">окна пвх - 0
+пластиковые окна - 4
+</t>
+        </is>
+      </c>
       <c r="C99" s="6" t="n">
         <v>2</v>
       </c>
@@ -3049,7 +3553,13 @@
           <t>Краснодарский край, Новолабинская</t>
         </is>
       </c>
-      <c r="B101" s="4" t="n"/>
+      <c r="B101" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">окна пвх - 0
+пластиковые окна - 2
+</t>
+        </is>
+      </c>
       <c r="C101" s="6" t="n">
         <v>14</v>
       </c>

</xml_diff>